<commit_message>
Fix pop up detail
</commit_message>
<xml_diff>
--- a/public/template/excel/format_laporan_operasi_2021_preview_new.xlsx
+++ b/public/template/excel/format_laporan_operasi_2021_preview_new.xlsx
@@ -1312,7 +1312,7 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
     <xf numFmtId="41" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="94">
+  <cellXfs count="95">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -1557,6 +1557,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1865,10 +1868,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H426"/>
+  <dimension ref="A1:H435"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A393" zoomScale="90" zoomScaleNormal="90" zoomScaleSheetLayoutView="178" zoomScalePageLayoutView="90" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView tabSelected="1" topLeftCell="A411" zoomScale="90" zoomScaleNormal="90" zoomScaleSheetLayoutView="178" zoomScalePageLayoutView="90" workbookViewId="0">
+      <selection activeCell="E435" sqref="E435:F435"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -11343,8 +11346,28 @@
         <v>58</v>
       </c>
     </row>
+    <row r="428" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E428" s="94"/>
+      <c r="F428" s="94"/>
+    </row>
+    <row r="429" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E429" s="94"/>
+      <c r="F429" s="94"/>
+    </row>
+    <row r="434" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="E434" s="94"/>
+      <c r="F434" s="94"/>
+    </row>
+    <row r="435" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="E435" s="94"/>
+      <c r="F435" s="94"/>
+    </row>
   </sheetData>
-  <mergeCells count="6">
+  <mergeCells count="10">
+    <mergeCell ref="E428:F428"/>
+    <mergeCell ref="E429:F429"/>
+    <mergeCell ref="E434:F434"/>
+    <mergeCell ref="E435:F435"/>
     <mergeCell ref="A9:G9"/>
     <mergeCell ref="A10:A11"/>
     <mergeCell ref="B10:B11"/>

</xml_diff>